<commit_message>
change WACC to 5%, comment out plot in scenario
</commit_message>
<xml_diff>
--- a/Data/Economics_Data.xlsx
+++ b/Data/Economics_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mathias/Desktop/pull from github/Thesis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE68830-CF8E-D540-A7EC-C9021631C927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1292EC5-7315-714C-966E-102D2532E767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6380" yWindow="3360" windowWidth="19220" windowHeight="11800" xr2:uid="{3BAE7179-B466-434C-BE96-56EBC5E2E167}"/>
   </bookViews>
@@ -95,13 +95,13 @@
     <t>discount rate</t>
   </si>
   <si>
-    <t>0.04</t>
-  </si>
-  <si>
     <t>Grid_Connection</t>
   </si>
   <si>
     <t>15.4552</t>
+  </si>
+  <si>
+    <t>0.05</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -499,7 +499,7 @@
         <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>16</v>
@@ -534,13 +534,13 @@
         <v>15</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>